<commit_message>
Games are extracted. Needs to be tested more
</commit_message>
<xml_diff>
--- a/SteamLibrary/TestExcel.xlsx
+++ b/SteamLibrary/TestExcel.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <x:si>
     <x:t>Game Title</x:t>
   </x:si>
@@ -78,6 +78,96 @@
   </x:si>
   <x:si>
     <x:t>War Thunder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>King of the Board</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Witches x Warlocks</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sector's Edge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>仙剑奇侠传九野</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Siren Head: Awakening</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Happy's Humble Burger Farm Alpha</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Last Spell: Prologue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LA Monsters</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GOD OF FLAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Farmer And Tree</x:t>
+  </x:si>
+  <x:si>
+    <x:t>World of Soccer RELOADED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Warlock Bentspine - Toilet Edition</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Greed Knights</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Card Blitz: WWII</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ratten Reich - Dance of Kings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oasis VR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shotgun Witch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MannaRites</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tree Trunk Brook</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chaos Combat Chess</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aimi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zero IDLE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scribble It!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Blood of Steel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Circle of Sumo: Online Rumble!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WKSP Rumble</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VR Only Binaural Odyssey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vecter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RuneScape ®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Eternal Return: Black Survival</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -563,7 +653,350 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1"/>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="A11" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="A17" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="A18" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="A19" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="A20" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B20" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="A21" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B21" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C21" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B22" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C22" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B23" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C23" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B27" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C27" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B30" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C30" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B31" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C31" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated and tested all workflows for add game process
</commit_message>
<xml_diff>
--- a/SteamLibrary/TestExcel.xlsx
+++ b/SteamLibrary/TestExcel.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <x:si>
     <x:t>Game Title</x:t>
   </x:si>
@@ -80,94 +80,91 @@
     <x:t>War Thunder</x:t>
   </x:si>
   <x:si>
-    <x:t>King of the Board</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Witches x Warlocks</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sector's Edge</x:t>
-  </x:si>
-  <x:si>
-    <x:t>仙剑奇侠传九野</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Siren Head: Awakening</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Happy's Humble Burger Farm Alpha</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Last Spell: Prologue</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LA Monsters</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GOD OF FLAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Farmer And Tree</x:t>
-  </x:si>
-  <x:si>
-    <x:t>World of Soccer RELOADED</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Warlock Bentspine - Toilet Edition</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Greed Knights</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Card Blitz: WWII</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ratten Reich - Dance of Kings</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oasis VR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shotgun Witch</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MannaRites</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tree Trunk Brook</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chaos Combat Chess</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Aimi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zero IDLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Scribble It!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blood of Steel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Circle of Sumo: Online Rumble!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WKSP Rumble</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VR Only Binaural Odyssey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vecter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RuneScape ®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Eternal Return: Black Survival</x:t>
+    <x:t>Toast Defense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tiny Toy Tanks</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BatuGame</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phobos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aurora: A Child's Journey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Verse Surf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Super Buckyball Tournament Preseason</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daikaiju Daikessen: Versus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Our Life: Beginnings &amp; Always</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Astria</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disc Space</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beat Me! - Puppetonia Tournament</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tribal Wars</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GranAge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Arc Apellago</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Swing Dunk (Open Beta)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Perfect Vermin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lawyer Guy: Defender of Justice</x:t>
+  </x:si>
+  <x:si>
+    <x:t>How Stories Die</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coloring Book for Adults</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apex Legends™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jendo: Origins</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Space Commander: War and Trade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chess'Extra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sword of the Necromancer - Prologue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SpellForce 3: Versus Edition</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Remnants</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Battle Star</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cubiscape 2</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -834,7 +831,7 @@
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B17" s="2" t="s">
         <x:v>9</x:v>
@@ -845,7 +842,7 @@
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="2" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B18" s="2" t="s">
         <x:v>9</x:v>
@@ -856,7 +853,7 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B19" s="2" t="s">
         <x:v>9</x:v>
@@ -867,7 +864,7 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B20" s="2" t="s">
         <x:v>9</x:v>
@@ -878,7 +875,7 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="2" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B21" s="2" t="s">
         <x:v>9</x:v>
@@ -889,7 +886,7 @@
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B22" s="2" t="s">
         <x:v>9</x:v>
@@ -900,7 +897,7 @@
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B23" s="2" t="s">
         <x:v>9</x:v>
@@ -911,7 +908,7 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="2" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B24" s="2" t="s">
         <x:v>9</x:v>
@@ -922,7 +919,7 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B25" s="2" t="s">
         <x:v>9</x:v>
@@ -933,7 +930,7 @@
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="A26" s="2" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B26" s="2" t="s">
         <x:v>9</x:v>
@@ -944,7 +941,7 @@
     </x:row>
     <x:row r="27" spans="1:4">
       <x:c r="A27" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B27" s="2" t="s">
         <x:v>9</x:v>
@@ -955,7 +952,7 @@
     </x:row>
     <x:row r="28" spans="1:4">
       <x:c r="A28" s="2" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B28" s="2" t="s">
         <x:v>9</x:v>
@@ -966,7 +963,7 @@
     </x:row>
     <x:row r="29" spans="1:4">
       <x:c r="A29" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B29" s="2" t="s">
         <x:v>9</x:v>
@@ -977,7 +974,7 @@
     </x:row>
     <x:row r="30" spans="1:4">
       <x:c r="A30" s="2" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B30" s="2" t="s">
         <x:v>9</x:v>
@@ -988,7 +985,7 @@
     </x:row>
     <x:row r="31" spans="1:4">
       <x:c r="A31" s="2" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B31" s="2" t="s">
         <x:v>9</x:v>

</xml_diff>

<commit_message>
Implemented functionality to install games from Steam Library
</commit_message>
<xml_diff>
--- a/SteamLibrary/TestExcel.xlsx
+++ b/SteamLibrary/TestExcel.xlsx
@@ -5,16 +5,17 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Documents\UiPath\GameGetterTemp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Documents\Revature\Team3-P2\SteamLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89113B-27D3-47C9-A639-737A8ED8DC56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0798D5D2-2D41-40B1-8E00-7B123E2EF014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="4830" yWindow="8850" windowWidth="16110" windowHeight="11235" firstSheet="0" activeTab="0" xr2:uid="{634990EF-350C-49C4-BE60-5843BCD391AF}"/>
+    <x:workbookView xWindow="16065" yWindow="2490" windowWidth="16110" windowHeight="11235" firstSheet="0" activeTab="2" xr2:uid="{634990EF-350C-49C4-BE60-5843BCD391AF}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="FreeGames" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="AddGames" sheetId="4" r:id="rId2"/>
+    <x:sheet name="InstallGames" sheetId="5" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191029"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Game Title</x:t>
   </x:si>
@@ -47,37 +48,34 @@
     <x:t>Install</x:t>
   </x:si>
   <x:si>
+    <x:t>Apex Legends</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phantasy Star Online 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Destiny 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>War Thunder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Assassin's Creed Odyssey</x:t>
+  </x:si>
+  <x:si>
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>Note</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Apex Legends</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yes</x:t>
-  </x:si>
-  <x:si>
     <x:t>Already In Library</x:t>
   </x:si>
   <x:si>
-    <x:t>Phantasy Star Online 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Need to handle age warning with exceptions</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Destiny 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Already added to library, should be handled with exceptions</x:t>
-  </x:si>
-  <x:si>
-    <x:t>War Thunder</x:t>
+    <x:t>Game Installing</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -449,20 +447,19 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E5"/>
+  <x:dimension ref="A1:D6"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E15" sqref="E15 E15:E15"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="F15" sqref="F15 F15:F15"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
     <x:col min="2" max="4" width="10.710938" style="2" customWidth="1"/>
-    <x:col min="5" max="5" width="55.855469" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -472,75 +469,63 @@
       <x:c r="C1" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="B2" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="2" t="s">
+      <x:c r="C2" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D2" s="2" t="s">
+      <x:c r="B3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="2" t="s">
+      <x:c r="B4" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="B5" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E3" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="2" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B4" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C4" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D4" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E4" s="2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B5" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C5" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="E15" s="2" t="s"/>
-    </x:row>
+      <x:c r="B6" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -551,19 +536,98 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{626652B7-649F-411A-A8E0-767C593B70A1}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{E2067B58-67F2-4A79-9F8E-90CD5D0BFCC2}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:B4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 A1:A1 A1:XFD1"/>
+      <x:selection activeCell="D24" sqref="D24 D24:D24"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="10.710938" style="2" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1"/>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{CE46C121-DF80-45DA-96AD-14ED91707A12}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="D7" sqref="D7 D7:D7"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="10.710938" style="2" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated game extraction to remove trademarks
</commit_message>
<xml_diff>
--- a/SteamLibrary/TestExcel.xlsx
+++ b/SteamLibrary/TestExcel.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <x:si>
     <x:t>Game Title</x:t>
   </x:si>
@@ -78,6 +78,9 @@
   </x:si>
   <x:si>
     <x:t>War Thunder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SUPERCHICOS</x:t>
   </x:si>
   <x:si>
     <x:t>Toast Defense</x:t>
@@ -831,7 +834,7 @@
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="2" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B17" s="2" t="s">
         <x:v>9</x:v>
@@ -842,7 +845,7 @@
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B18" s="2" t="s">
         <x:v>9</x:v>
@@ -853,7 +856,7 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="2" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B19" s="2" t="s">
         <x:v>9</x:v>
@@ -864,7 +867,7 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B20" s="2" t="s">
         <x:v>9</x:v>
@@ -875,7 +878,7 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B21" s="2" t="s">
         <x:v>9</x:v>
@@ -886,7 +889,7 @@
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="2" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B22" s="2" t="s">
         <x:v>9</x:v>
@@ -897,7 +900,7 @@
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B23" s="2" t="s">
         <x:v>9</x:v>
@@ -908,7 +911,7 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B24" s="2" t="s">
         <x:v>9</x:v>
@@ -919,7 +922,7 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="2" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B25" s="2" t="s">
         <x:v>9</x:v>
@@ -930,7 +933,7 @@
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="A26" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B26" s="2" t="s">
         <x:v>9</x:v>
@@ -941,7 +944,7 @@
     </x:row>
     <x:row r="27" spans="1:4">
       <x:c r="A27" s="2" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B27" s="2" t="s">
         <x:v>9</x:v>
@@ -952,7 +955,7 @@
     </x:row>
     <x:row r="28" spans="1:4">
       <x:c r="A28" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B28" s="2" t="s">
         <x:v>9</x:v>
@@ -963,7 +966,7 @@
     </x:row>
     <x:row r="29" spans="1:4">
       <x:c r="A29" s="2" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B29" s="2" t="s">
         <x:v>9</x:v>
@@ -974,7 +977,7 @@
     </x:row>
     <x:row r="30" spans="1:4">
       <x:c r="A30" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B30" s="2" t="s">
         <x:v>9</x:v>
@@ -985,7 +988,7 @@
     </x:row>
     <x:row r="31" spans="1:4">
       <x:c r="A31" s="2" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B31" s="2" t="s">
         <x:v>9</x:v>

</xml_diff>

<commit_message>
Removed trademarks from extracted games
</commit_message>
<xml_diff>
--- a/SteamLibrary/TestExcel.xlsx
+++ b/SteamLibrary/TestExcel.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <x:si>
     <x:t>Game Title</x:t>
   </x:si>
@@ -143,9 +143,6 @@
     <x:t>Coloring Book for Adults</x:t>
   </x:si>
   <x:si>
-    <x:t>Apex Legends™</x:t>
-  </x:si>
-  <x:si>
     <x:t>Jendo: Origins</x:t>
   </x:si>
   <x:si>
@@ -167,7 +164,7 @@
     <x:t>Battle Star</x:t>
   </x:si>
   <x:si>
-    <x:t>Cubiscape 2</x:t>
+    <x:t>Strategy, Turn-Based Strategy, JRPG, Roguelite</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -834,7 +831,7 @@
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B17" s="2" t="s">
         <x:v>9</x:v>
@@ -845,7 +842,7 @@
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="2" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B18" s="2" t="s">
         <x:v>9</x:v>
@@ -856,7 +853,7 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B19" s="2" t="s">
         <x:v>9</x:v>
@@ -867,7 +864,7 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B20" s="2" t="s">
         <x:v>9</x:v>
@@ -878,7 +875,7 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="2" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B21" s="2" t="s">
         <x:v>9</x:v>
@@ -889,7 +886,7 @@
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B22" s="2" t="s">
         <x:v>9</x:v>
@@ -900,7 +897,7 @@
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B23" s="2" t="s">
         <x:v>9</x:v>
@@ -911,7 +908,7 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="2" t="s">
-        <x:v>36</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B24" s="2" t="s">
         <x:v>9</x:v>
@@ -922,7 +919,7 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B25" s="2" t="s">
         <x:v>9</x:v>
@@ -933,7 +930,7 @@
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="A26" s="2" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B26" s="2" t="s">
         <x:v>9</x:v>
@@ -944,7 +941,7 @@
     </x:row>
     <x:row r="27" spans="1:4">
       <x:c r="A27" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B27" s="2" t="s">
         <x:v>9</x:v>
@@ -955,7 +952,7 @@
     </x:row>
     <x:row r="28" spans="1:4">
       <x:c r="A28" s="2" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B28" s="2" t="s">
         <x:v>9</x:v>
@@ -966,7 +963,7 @@
     </x:row>
     <x:row r="29" spans="1:4">
       <x:c r="A29" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B29" s="2" t="s">
         <x:v>9</x:v>
@@ -977,7 +974,7 @@
     </x:row>
     <x:row r="30" spans="1:4">
       <x:c r="A30" s="2" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B30" s="2" t="s">
         <x:v>9</x:v>
@@ -988,12 +985,23 @@
     </x:row>
     <x:row r="31" spans="1:4">
       <x:c r="A31" s="2" t="s">
-        <x:v>43</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B31" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="C31" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B32" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C32" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>

</xml_diff>